<commit_message>
[*] check mold change
</commit_message>
<xml_diff>
--- a/Files/FlowDiagram_New.xlsx
+++ b/Files/FlowDiagram_New.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Autonics\changshin_apss\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Autonics\changshin_apss\APSS\APSS\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -963,7 +963,34 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -975,43 +1002,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -8302,7 +8302,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>check Mold Table</a:t>
+            <a:t>check Mold Change</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -8665,33 +8665,33 @@
       <c r="T1" s="29"/>
     </row>
     <row r="2" spans="2:20">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="61"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="52"/>
       <c r="F2" s="30"/>
       <c r="G2" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="61"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="52"/>
       <c r="K2" s="30"/>
       <c r="L2" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="61"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="52"/>
       <c r="P2" s="30"/>
       <c r="Q2" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="60"/>
-      <c r="S2" s="60"/>
-      <c r="T2" s="62"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="65"/>
     </row>
     <row r="3" spans="2:20">
       <c r="B3" s="16"/>
@@ -8715,89 +8715,89 @@
       <c r="T3" s="17"/>
     </row>
     <row r="4" spans="2:20">
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="56" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="54"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="51" t="s">
+      <c r="G4" s="60" t="s">
         <v>5</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="54" t="s">
+      <c r="I4" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="54"/>
+      <c r="J4" s="53"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="51" t="s">
+      <c r="L4" s="60" t="s">
         <v>5</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="54" t="s">
+      <c r="N4" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="54"/>
+      <c r="O4" s="53"/>
       <c r="P4" s="3"/>
-      <c r="Q4" s="51" t="s">
+      <c r="Q4" s="60" t="s">
         <v>5</v>
       </c>
       <c r="R4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="S4" s="54" t="s">
+      <c r="S4" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="T4" s="55"/>
+      <c r="T4" s="63"/>
     </row>
     <row r="5" spans="2:20">
-      <c r="B5" s="65"/>
+      <c r="B5" s="57"/>
       <c r="C5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="56" t="s">
+      <c r="D5" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="57"/>
+      <c r="E5" s="55"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="52"/>
+      <c r="G5" s="61"/>
       <c r="H5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="56" t="s">
+      <c r="I5" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="57"/>
+      <c r="J5" s="55"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="52"/>
+      <c r="L5" s="61"/>
       <c r="M5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="N5" s="56" t="s">
+      <c r="N5" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="O5" s="57"/>
+      <c r="O5" s="55"/>
       <c r="P5" s="3"/>
-      <c r="Q5" s="52"/>
+      <c r="Q5" s="61"/>
       <c r="R5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="S5" s="56" t="s">
+      <c r="S5" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="T5" s="58"/>
+      <c r="T5" s="64"/>
     </row>
     <row r="6" spans="2:20">
-      <c r="B6" s="65"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="5"/>
       <c r="D6" s="1" t="s">
         <v>6</v>
@@ -8806,7 +8806,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="52"/>
+      <c r="G6" s="61"/>
       <c r="H6" s="5"/>
       <c r="I6" s="1" t="s">
         <v>6</v>
@@ -8815,7 +8815,7 @@
         <v>7</v>
       </c>
       <c r="K6" s="3"/>
-      <c r="L6" s="52"/>
+      <c r="L6" s="61"/>
       <c r="M6" s="5"/>
       <c r="N6" s="1" t="s">
         <v>6</v>
@@ -8824,7 +8824,7 @@
         <v>7</v>
       </c>
       <c r="P6" s="3"/>
-      <c r="Q6" s="52"/>
+      <c r="Q6" s="61"/>
       <c r="R6" s="5"/>
       <c r="S6" s="1" t="s">
         <v>6</v>
@@ -8834,7 +8834,7 @@
       </c>
     </row>
     <row r="7" spans="2:20">
-      <c r="B7" s="65"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="5" t="s">
         <v>2</v>
       </c>
@@ -8845,7 +8845,7 @@
         <v>600</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="52"/>
+      <c r="G7" s="61"/>
       <c r="H7" s="5" t="s">
         <v>2</v>
       </c>
@@ -8856,7 +8856,7 @@
         <v>602</v>
       </c>
       <c r="K7" s="3"/>
-      <c r="L7" s="52"/>
+      <c r="L7" s="61"/>
       <c r="M7" s="5" t="s">
         <v>2</v>
       </c>
@@ -8867,7 +8867,7 @@
         <v>604</v>
       </c>
       <c r="P7" s="3"/>
-      <c r="Q7" s="52"/>
+      <c r="Q7" s="61"/>
       <c r="R7" s="5" t="s">
         <v>2</v>
       </c>
@@ -8879,7 +8879,7 @@
       </c>
     </row>
     <row r="8" spans="2:20">
-      <c r="B8" s="65"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="5" t="s">
         <v>3</v>
       </c>
@@ -8890,7 +8890,7 @@
         <v>119</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="52"/>
+      <c r="G8" s="61"/>
       <c r="H8" s="5" t="s">
         <v>3</v>
       </c>
@@ -8901,7 +8901,7 @@
         <v>179</v>
       </c>
       <c r="K8" s="3"/>
-      <c r="L8" s="52"/>
+      <c r="L8" s="61"/>
       <c r="M8" s="5" t="s">
         <v>3</v>
       </c>
@@ -8912,7 +8912,7 @@
         <v>239</v>
       </c>
       <c r="P8" s="3"/>
-      <c r="Q8" s="52"/>
+      <c r="Q8" s="61"/>
       <c r="R8" s="5" t="s">
         <v>3</v>
       </c>
@@ -8924,7 +8924,7 @@
       </c>
     </row>
     <row r="9" spans="2:20">
-      <c r="B9" s="65"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="5" t="s">
         <v>4</v>
       </c>
@@ -8935,7 +8935,7 @@
         <v>121</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="52"/>
+      <c r="G9" s="61"/>
       <c r="H9" s="5" t="s">
         <v>4</v>
       </c>
@@ -8946,7 +8946,7 @@
         <v>181</v>
       </c>
       <c r="K9" s="3"/>
-      <c r="L9" s="52"/>
+      <c r="L9" s="61"/>
       <c r="M9" s="5" t="s">
         <v>4</v>
       </c>
@@ -8957,7 +8957,7 @@
         <v>241</v>
       </c>
       <c r="P9" s="3"/>
-      <c r="Q9" s="52"/>
+      <c r="Q9" s="61"/>
       <c r="R9" s="5" t="s">
         <v>4</v>
       </c>
@@ -8969,28 +8969,28 @@
       </c>
     </row>
     <row r="10" spans="2:20">
-      <c r="B10" s="65"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="4"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="52"/>
+      <c r="G10" s="61"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="4"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="52"/>
+      <c r="L10" s="61"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="4"/>
       <c r="P10" s="3"/>
-      <c r="Q10" s="52"/>
+      <c r="Q10" s="61"/>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
       <c r="T10" s="17"/>
     </row>
     <row r="11" spans="2:20">
-      <c r="B11" s="65"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="6" t="s">
         <v>9</v>
       </c>
@@ -8999,7 +8999,7 @@
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="52"/>
+      <c r="G11" s="61"/>
       <c r="H11" s="6" t="s">
         <v>9</v>
       </c>
@@ -9008,7 +9008,7 @@
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="52"/>
+      <c r="L11" s="61"/>
       <c r="M11" s="6" t="s">
         <v>9</v>
       </c>
@@ -9017,7 +9017,7 @@
       </c>
       <c r="O11" s="8"/>
       <c r="P11" s="3"/>
-      <c r="Q11" s="52"/>
+      <c r="Q11" s="61"/>
       <c r="R11" s="6" t="s">
         <v>9</v>
       </c>
@@ -9027,7 +9027,7 @@
       <c r="T11" s="21"/>
     </row>
     <row r="12" spans="2:20">
-      <c r="B12" s="66"/>
+      <c r="B12" s="58"/>
       <c r="C12" s="9" t="s">
         <v>25</v>
       </c>
@@ -9038,7 +9038,7 @@
         <v>24</v>
       </c>
       <c r="F12" s="3"/>
-      <c r="G12" s="53"/>
+      <c r="G12" s="62"/>
       <c r="H12" s="9" t="s">
         <v>25</v>
       </c>
@@ -9049,7 +9049,7 @@
         <v>24</v>
       </c>
       <c r="K12" s="3"/>
-      <c r="L12" s="53"/>
+      <c r="L12" s="62"/>
       <c r="M12" s="9" t="s">
         <v>25</v>
       </c>
@@ -9060,7 +9060,7 @@
         <v>24</v>
       </c>
       <c r="P12" s="3"/>
-      <c r="Q12" s="53"/>
+      <c r="Q12" s="62"/>
       <c r="R12" s="9" t="s">
         <v>25</v>
       </c>
@@ -9093,89 +9093,89 @@
       <c r="T13" s="17"/>
     </row>
     <row r="14" spans="2:20">
-      <c r="B14" s="64" t="s">
+      <c r="B14" s="56" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="54" t="s">
+      <c r="D14" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="54"/>
+      <c r="E14" s="53"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="51" t="s">
+      <c r="G14" s="60" t="s">
         <v>11</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="I14" s="54" t="s">
+      <c r="I14" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="54"/>
+      <c r="J14" s="53"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="51" t="s">
+      <c r="L14" s="60" t="s">
         <v>11</v>
       </c>
       <c r="M14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="N14" s="54" t="s">
+      <c r="N14" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="O14" s="54"/>
+      <c r="O14" s="53"/>
       <c r="P14" s="3"/>
-      <c r="Q14" s="51" t="s">
+      <c r="Q14" s="60" t="s">
         <v>11</v>
       </c>
       <c r="R14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="S14" s="54" t="s">
+      <c r="S14" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="T14" s="55"/>
+      <c r="T14" s="63"/>
     </row>
     <row r="15" spans="2:20">
-      <c r="B15" s="65"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="56" t="s">
+      <c r="D15" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="57"/>
+      <c r="E15" s="55"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="52"/>
+      <c r="G15" s="61"/>
       <c r="H15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I15" s="56" t="s">
+      <c r="I15" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="57"/>
+      <c r="J15" s="55"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="52"/>
+      <c r="L15" s="61"/>
       <c r="M15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="N15" s="56" t="s">
+      <c r="N15" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="O15" s="57"/>
+      <c r="O15" s="55"/>
       <c r="P15" s="3"/>
-      <c r="Q15" s="52"/>
+      <c r="Q15" s="61"/>
       <c r="R15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="S15" s="56" t="s">
+      <c r="S15" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="T15" s="58"/>
+      <c r="T15" s="64"/>
     </row>
     <row r="16" spans="2:20">
-      <c r="B16" s="65"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="5"/>
       <c r="D16" s="1" t="s">
         <v>6</v>
@@ -9184,7 +9184,7 @@
         <v>7</v>
       </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="52"/>
+      <c r="G16" s="61"/>
       <c r="H16" s="5"/>
       <c r="I16" s="1" t="s">
         <v>6</v>
@@ -9193,7 +9193,7 @@
         <v>7</v>
       </c>
       <c r="K16" s="3"/>
-      <c r="L16" s="52"/>
+      <c r="L16" s="61"/>
       <c r="M16" s="5"/>
       <c r="N16" s="1" t="s">
         <v>6</v>
@@ -9202,7 +9202,7 @@
         <v>7</v>
       </c>
       <c r="P16" s="3"/>
-      <c r="Q16" s="52"/>
+      <c r="Q16" s="61"/>
       <c r="R16" s="5"/>
       <c r="S16" s="1" t="s">
         <v>6</v>
@@ -9212,7 +9212,7 @@
       </c>
     </row>
     <row r="17" spans="2:20">
-      <c r="B17" s="65"/>
+      <c r="B17" s="57"/>
       <c r="C17" s="5" t="s">
         <v>2</v>
       </c>
@@ -9223,7 +9223,7 @@
         <v>601</v>
       </c>
       <c r="F17" s="3"/>
-      <c r="G17" s="52"/>
+      <c r="G17" s="61"/>
       <c r="H17" s="5" t="s">
         <v>2</v>
       </c>
@@ -9234,7 +9234,7 @@
         <v>603</v>
       </c>
       <c r="K17" s="3"/>
-      <c r="L17" s="52"/>
+      <c r="L17" s="61"/>
       <c r="M17" s="5" t="s">
         <v>2</v>
       </c>
@@ -9245,7 +9245,7 @@
         <v>605</v>
       </c>
       <c r="P17" s="3"/>
-      <c r="Q17" s="52"/>
+      <c r="Q17" s="61"/>
       <c r="R17" s="5" t="s">
         <v>2</v>
       </c>
@@ -9257,7 +9257,7 @@
       </c>
     </row>
     <row r="18" spans="2:20">
-      <c r="B18" s="65"/>
+      <c r="B18" s="57"/>
       <c r="C18" s="5" t="s">
         <v>3</v>
       </c>
@@ -9268,7 +9268,7 @@
         <v>149</v>
       </c>
       <c r="F18" s="3"/>
-      <c r="G18" s="52"/>
+      <c r="G18" s="61"/>
       <c r="H18" s="5" t="s">
         <v>3</v>
       </c>
@@ -9279,7 +9279,7 @@
         <v>209</v>
       </c>
       <c r="K18" s="3"/>
-      <c r="L18" s="52"/>
+      <c r="L18" s="61"/>
       <c r="M18" s="5" t="s">
         <v>3</v>
       </c>
@@ -9290,7 +9290,7 @@
         <v>269</v>
       </c>
       <c r="P18" s="3"/>
-      <c r="Q18" s="52"/>
+      <c r="Q18" s="61"/>
       <c r="R18" s="5" t="s">
         <v>3</v>
       </c>
@@ -9302,7 +9302,7 @@
       </c>
     </row>
     <row r="19" spans="2:20">
-      <c r="B19" s="65"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="5" t="s">
         <v>4</v>
       </c>
@@ -9313,7 +9313,7 @@
         <v>151</v>
       </c>
       <c r="F19" s="3"/>
-      <c r="G19" s="52"/>
+      <c r="G19" s="61"/>
       <c r="H19" s="5" t="s">
         <v>4</v>
       </c>
@@ -9324,7 +9324,7 @@
         <v>211</v>
       </c>
       <c r="K19" s="3"/>
-      <c r="L19" s="52"/>
+      <c r="L19" s="61"/>
       <c r="M19" s="5" t="s">
         <v>4</v>
       </c>
@@ -9335,7 +9335,7 @@
         <v>271</v>
       </c>
       <c r="P19" s="3"/>
-      <c r="Q19" s="52"/>
+      <c r="Q19" s="61"/>
       <c r="R19" s="5" t="s">
         <v>4</v>
       </c>
@@ -9347,28 +9347,28 @@
       </c>
     </row>
     <row r="20" spans="2:20">
-      <c r="B20" s="65"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="4"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="52"/>
+      <c r="G20" s="61"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="4"/>
       <c r="K20" s="3"/>
-      <c r="L20" s="52"/>
+      <c r="L20" s="61"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="4"/>
       <c r="P20" s="3"/>
-      <c r="Q20" s="52"/>
+      <c r="Q20" s="61"/>
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
       <c r="T20" s="17"/>
     </row>
     <row r="21" spans="2:20">
-      <c r="B21" s="65"/>
+      <c r="B21" s="57"/>
       <c r="C21" s="6" t="s">
         <v>9</v>
       </c>
@@ -9377,7 +9377,7 @@
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="52"/>
+      <c r="G21" s="61"/>
       <c r="H21" s="6" t="s">
         <v>9</v>
       </c>
@@ -9386,7 +9386,7 @@
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="3"/>
-      <c r="L21" s="52"/>
+      <c r="L21" s="61"/>
       <c r="M21" s="6" t="s">
         <v>9</v>
       </c>
@@ -9395,7 +9395,7 @@
       </c>
       <c r="O21" s="8"/>
       <c r="P21" s="3"/>
-      <c r="Q21" s="52"/>
+      <c r="Q21" s="61"/>
       <c r="R21" s="6" t="s">
         <v>9</v>
       </c>
@@ -9405,7 +9405,7 @@
       <c r="T21" s="21"/>
     </row>
     <row r="22" spans="2:20">
-      <c r="B22" s="66"/>
+      <c r="B22" s="58"/>
       <c r="C22" s="9" t="s">
         <v>25</v>
       </c>
@@ -9416,7 +9416,7 @@
         <v>24</v>
       </c>
       <c r="F22" s="3"/>
-      <c r="G22" s="53"/>
+      <c r="G22" s="62"/>
       <c r="H22" s="9" t="s">
         <v>25</v>
       </c>
@@ -9427,7 +9427,7 @@
         <v>24</v>
       </c>
       <c r="K22" s="3"/>
-      <c r="L22" s="53"/>
+      <c r="L22" s="62"/>
       <c r="M22" s="9" t="s">
         <v>25</v>
       </c>
@@ -9438,7 +9438,7 @@
         <v>24</v>
       </c>
       <c r="P22" s="3"/>
-      <c r="Q22" s="53"/>
+      <c r="Q22" s="62"/>
       <c r="R22" s="9" t="s">
         <v>25</v>
       </c>
@@ -9817,11 +9817,11 @@
       <c r="N39" s="49">
         <v>1</v>
       </c>
-      <c r="O39" s="50" t="s">
+      <c r="O39" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="P39" s="50"/>
-      <c r="Q39" s="50"/>
+      <c r="P39" s="66"/>
+      <c r="Q39" s="66"/>
     </row>
     <row r="40" spans="3:17">
       <c r="H40" s="38" t="s">
@@ -9839,11 +9839,11 @@
       <c r="N40" s="49">
         <v>2</v>
       </c>
-      <c r="O40" s="50" t="s">
+      <c r="O40" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="P40" s="50"/>
-      <c r="Q40" s="50"/>
+      <c r="P40" s="66"/>
+      <c r="Q40" s="66"/>
     </row>
     <row r="41" spans="3:17">
       <c r="H41" s="38"/>
@@ -9859,11 +9859,11 @@
       <c r="N41" s="49">
         <v>3</v>
       </c>
-      <c r="O41" s="50" t="s">
+      <c r="O41" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="P41" s="50"/>
-      <c r="Q41" s="50"/>
+      <c r="P41" s="66"/>
+      <c r="Q41" s="66"/>
     </row>
     <row r="42" spans="3:17">
       <c r="H42" s="47" t="s">
@@ -9913,20 +9913,12 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B4:B12"/>
-    <mergeCell ref="B14:B22"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="G4:G12"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="G14:G22"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="O39:Q39"/>
+    <mergeCell ref="O40:Q40"/>
+    <mergeCell ref="O41:Q41"/>
+    <mergeCell ref="L14:L22"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="Q14:Q22"/>
     <mergeCell ref="S14:T14"/>
     <mergeCell ref="N15:O15"/>
     <mergeCell ref="S15:T15"/>
@@ -9938,12 +9930,20 @@
     <mergeCell ref="S4:T4"/>
     <mergeCell ref="N5:O5"/>
     <mergeCell ref="S5:T5"/>
-    <mergeCell ref="O39:Q39"/>
-    <mergeCell ref="O40:Q40"/>
-    <mergeCell ref="O41:Q41"/>
-    <mergeCell ref="L14:L22"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="Q14:Q22"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="G4:G12"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="G14:G22"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B4:B12"/>
+    <mergeCell ref="B14:B22"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9956,7 +9956,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>

</xml_diff>

<commit_message>
[*] modify Auto/Manual value
</commit_message>
<xml_diff>
--- a/Files/FlowDiagram_New.xlsx
+++ b/Files/FlowDiagram_New.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="90" windowWidth="14325" windowHeight="8640" activeTab="2"/>
+    <workbookView xWindow="1035" yWindow="90" windowWidth="14325" windowHeight="8640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="82">
   <si>
     <t>Mold</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -314,6 +314,14 @@
   </si>
   <si>
     <t>holiday</t>
+  </si>
+  <si>
+    <t>0-Auto</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-Manual</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -8625,10 +8633,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:T45"/>
+  <dimension ref="B1:T49"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38:J45"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -9909,6 +9917,19 @@
       </c>
       <c r="J45" s="38" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="3:17">
+      <c r="C48" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4">
+      <c r="D49" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -9955,7 +9976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A30" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[*] barcode read some fix
</commit_message>
<xml_diff>
--- a/Files/FlowDiagram_New.xlsx
+++ b/Files/FlowDiagram_New.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Autonics\changshin_apss\APSS\APSS\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ITSupport\Desktop\changshin_factory2\APSS\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="84">
   <si>
     <t>Mold</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -323,6 +323,12 @@
     <t>1-Manual</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>0-OFF</t>
+  </si>
+  <si>
+    <t>1-Blinking</t>
+  </si>
 </sst>
 </file>
 
@@ -332,7 +338,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -340,14 +346,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -355,7 +361,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -364,14 +370,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -971,7 +977,34 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -980,13 +1013,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -998,33 +1028,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -8623,7 +8629,7 @@
       <selection activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8635,23 +8641,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="1.875" customWidth="1"/>
+    <col min="1" max="1" width="1.85546875" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="6" max="6" width="2" customWidth="1"/>
-    <col min="8" max="8" width="13.125" customWidth="1"/>
-    <col min="11" max="11" width="2.875" customWidth="1"/>
-    <col min="13" max="13" width="13.125" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="2.85546875" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" customWidth="1"/>
     <col min="16" max="16" width="2" customWidth="1"/>
-    <col min="18" max="18" width="13.125" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="17.25" thickBot="1">
+    <row r="1" spans="2:20" ht="15.75" thickBot="1">
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
       <c r="D1" s="29"/>
@@ -8673,33 +8679,33 @@
       <c r="T1" s="29"/>
     </row>
     <row r="2" spans="2:20">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="52"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="61"/>
       <c r="F2" s="30"/>
       <c r="G2" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="52"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="61"/>
       <c r="K2" s="30"/>
       <c r="L2" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="52"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="61"/>
       <c r="P2" s="30"/>
       <c r="Q2" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="65"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="62"/>
     </row>
     <row r="3" spans="2:20">
       <c r="B3" s="16"/>
@@ -8723,89 +8729,89 @@
       <c r="T3" s="17"/>
     </row>
     <row r="4" spans="2:20">
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="64" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="53" t="s">
+      <c r="D4" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="53"/>
+      <c r="E4" s="54"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="51" t="s">
         <v>5</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="53" t="s">
+      <c r="I4" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="53"/>
+      <c r="J4" s="54"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="60" t="s">
+      <c r="L4" s="51" t="s">
         <v>5</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="53" t="s">
+      <c r="N4" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="53"/>
+      <c r="O4" s="54"/>
       <c r="P4" s="3"/>
-      <c r="Q4" s="60" t="s">
+      <c r="Q4" s="51" t="s">
         <v>5</v>
       </c>
       <c r="R4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="S4" s="53" t="s">
+      <c r="S4" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="T4" s="63"/>
+      <c r="T4" s="55"/>
     </row>
     <row r="5" spans="2:20">
-      <c r="B5" s="57"/>
+      <c r="B5" s="65"/>
       <c r="C5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="55"/>
+      <c r="E5" s="57"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="61"/>
+      <c r="G5" s="52"/>
       <c r="H5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="54" t="s">
+      <c r="I5" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="55"/>
+      <c r="J5" s="57"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="61"/>
+      <c r="L5" s="52"/>
       <c r="M5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="N5" s="54" t="s">
+      <c r="N5" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="O5" s="55"/>
+      <c r="O5" s="57"/>
       <c r="P5" s="3"/>
-      <c r="Q5" s="61"/>
+      <c r="Q5" s="52"/>
       <c r="R5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="S5" s="54" t="s">
+      <c r="S5" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="T5" s="64"/>
+      <c r="T5" s="58"/>
     </row>
     <row r="6" spans="2:20">
-      <c r="B6" s="57"/>
+      <c r="B6" s="65"/>
       <c r="C6" s="5"/>
       <c r="D6" s="1" t="s">
         <v>6</v>
@@ -8814,7 +8820,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="61"/>
+      <c r="G6" s="52"/>
       <c r="H6" s="5"/>
       <c r="I6" s="1" t="s">
         <v>6</v>
@@ -8823,7 +8829,7 @@
         <v>7</v>
       </c>
       <c r="K6" s="3"/>
-      <c r="L6" s="61"/>
+      <c r="L6" s="52"/>
       <c r="M6" s="5"/>
       <c r="N6" s="1" t="s">
         <v>6</v>
@@ -8832,7 +8838,7 @@
         <v>7</v>
       </c>
       <c r="P6" s="3"/>
-      <c r="Q6" s="61"/>
+      <c r="Q6" s="52"/>
       <c r="R6" s="5"/>
       <c r="S6" s="1" t="s">
         <v>6</v>
@@ -8842,7 +8848,7 @@
       </c>
     </row>
     <row r="7" spans="2:20">
-      <c r="B7" s="57"/>
+      <c r="B7" s="65"/>
       <c r="C7" s="5" t="s">
         <v>2</v>
       </c>
@@ -8853,7 +8859,7 @@
         <v>600</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="61"/>
+      <c r="G7" s="52"/>
       <c r="H7" s="5" t="s">
         <v>2</v>
       </c>
@@ -8864,7 +8870,7 @@
         <v>602</v>
       </c>
       <c r="K7" s="3"/>
-      <c r="L7" s="61"/>
+      <c r="L7" s="52"/>
       <c r="M7" s="5" t="s">
         <v>2</v>
       </c>
@@ -8875,7 +8881,7 @@
         <v>604</v>
       </c>
       <c r="P7" s="3"/>
-      <c r="Q7" s="61"/>
+      <c r="Q7" s="52"/>
       <c r="R7" s="5" t="s">
         <v>2</v>
       </c>
@@ -8887,7 +8893,7 @@
       </c>
     </row>
     <row r="8" spans="2:20">
-      <c r="B8" s="57"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="5" t="s">
         <v>3</v>
       </c>
@@ -8898,7 +8904,7 @@
         <v>119</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="61"/>
+      <c r="G8" s="52"/>
       <c r="H8" s="5" t="s">
         <v>3</v>
       </c>
@@ -8909,7 +8915,7 @@
         <v>179</v>
       </c>
       <c r="K8" s="3"/>
-      <c r="L8" s="61"/>
+      <c r="L8" s="52"/>
       <c r="M8" s="5" t="s">
         <v>3</v>
       </c>
@@ -8920,7 +8926,7 @@
         <v>239</v>
       </c>
       <c r="P8" s="3"/>
-      <c r="Q8" s="61"/>
+      <c r="Q8" s="52"/>
       <c r="R8" s="5" t="s">
         <v>3</v>
       </c>
@@ -8932,7 +8938,7 @@
       </c>
     </row>
     <row r="9" spans="2:20">
-      <c r="B9" s="57"/>
+      <c r="B9" s="65"/>
       <c r="C9" s="5" t="s">
         <v>4</v>
       </c>
@@ -8943,7 +8949,7 @@
         <v>121</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="61"/>
+      <c r="G9" s="52"/>
       <c r="H9" s="5" t="s">
         <v>4</v>
       </c>
@@ -8954,7 +8960,7 @@
         <v>181</v>
       </c>
       <c r="K9" s="3"/>
-      <c r="L9" s="61"/>
+      <c r="L9" s="52"/>
       <c r="M9" s="5" t="s">
         <v>4</v>
       </c>
@@ -8965,7 +8971,7 @@
         <v>241</v>
       </c>
       <c r="P9" s="3"/>
-      <c r="Q9" s="61"/>
+      <c r="Q9" s="52"/>
       <c r="R9" s="5" t="s">
         <v>4</v>
       </c>
@@ -8977,28 +8983,28 @@
       </c>
     </row>
     <row r="10" spans="2:20">
-      <c r="B10" s="57"/>
+      <c r="B10" s="65"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="4"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="61"/>
+      <c r="G10" s="52"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="4"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="61"/>
+      <c r="L10" s="52"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="4"/>
       <c r="P10" s="3"/>
-      <c r="Q10" s="61"/>
+      <c r="Q10" s="52"/>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
       <c r="T10" s="17"/>
     </row>
     <row r="11" spans="2:20">
-      <c r="B11" s="57"/>
+      <c r="B11" s="65"/>
       <c r="C11" s="6" t="s">
         <v>9</v>
       </c>
@@ -9007,7 +9013,7 @@
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="61"/>
+      <c r="G11" s="52"/>
       <c r="H11" s="6" t="s">
         <v>9</v>
       </c>
@@ -9016,7 +9022,7 @@
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="61"/>
+      <c r="L11" s="52"/>
       <c r="M11" s="6" t="s">
         <v>9</v>
       </c>
@@ -9025,7 +9031,7 @@
       </c>
       <c r="O11" s="8"/>
       <c r="P11" s="3"/>
-      <c r="Q11" s="61"/>
+      <c r="Q11" s="52"/>
       <c r="R11" s="6" t="s">
         <v>9</v>
       </c>
@@ -9035,7 +9041,7 @@
       <c r="T11" s="21"/>
     </row>
     <row r="12" spans="2:20">
-      <c r="B12" s="58"/>
+      <c r="B12" s="66"/>
       <c r="C12" s="9" t="s">
         <v>25</v>
       </c>
@@ -9046,7 +9052,7 @@
         <v>24</v>
       </c>
       <c r="F12" s="3"/>
-      <c r="G12" s="62"/>
+      <c r="G12" s="53"/>
       <c r="H12" s="9" t="s">
         <v>25</v>
       </c>
@@ -9057,7 +9063,7 @@
         <v>24</v>
       </c>
       <c r="K12" s="3"/>
-      <c r="L12" s="62"/>
+      <c r="L12" s="53"/>
       <c r="M12" s="9" t="s">
         <v>25</v>
       </c>
@@ -9068,7 +9074,7 @@
         <v>24</v>
       </c>
       <c r="P12" s="3"/>
-      <c r="Q12" s="62"/>
+      <c r="Q12" s="53"/>
       <c r="R12" s="9" t="s">
         <v>25</v>
       </c>
@@ -9101,89 +9107,89 @@
       <c r="T13" s="17"/>
     </row>
     <row r="14" spans="2:20">
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="64" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="53" t="s">
+      <c r="D14" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="53"/>
+      <c r="E14" s="54"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="60" t="s">
+      <c r="G14" s="51" t="s">
         <v>11</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="I14" s="53" t="s">
+      <c r="I14" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="53"/>
+      <c r="J14" s="54"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="60" t="s">
+      <c r="L14" s="51" t="s">
         <v>11</v>
       </c>
       <c r="M14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="N14" s="53" t="s">
+      <c r="N14" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="O14" s="53"/>
+      <c r="O14" s="54"/>
       <c r="P14" s="3"/>
-      <c r="Q14" s="60" t="s">
+      <c r="Q14" s="51" t="s">
         <v>11</v>
       </c>
       <c r="R14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="S14" s="53" t="s">
+      <c r="S14" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="T14" s="63"/>
+      <c r="T14" s="55"/>
     </row>
     <row r="15" spans="2:20">
-      <c r="B15" s="57"/>
+      <c r="B15" s="65"/>
       <c r="C15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="54" t="s">
+      <c r="D15" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="55"/>
+      <c r="E15" s="57"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="61"/>
+      <c r="G15" s="52"/>
       <c r="H15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I15" s="54" t="s">
+      <c r="I15" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="55"/>
+      <c r="J15" s="57"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="61"/>
+      <c r="L15" s="52"/>
       <c r="M15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="N15" s="54" t="s">
+      <c r="N15" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="O15" s="55"/>
+      <c r="O15" s="57"/>
       <c r="P15" s="3"/>
-      <c r="Q15" s="61"/>
+      <c r="Q15" s="52"/>
       <c r="R15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="S15" s="54" t="s">
+      <c r="S15" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="T15" s="64"/>
+      <c r="T15" s="58"/>
     </row>
     <row r="16" spans="2:20">
-      <c r="B16" s="57"/>
+      <c r="B16" s="65"/>
       <c r="C16" s="5"/>
       <c r="D16" s="1" t="s">
         <v>6</v>
@@ -9192,7 +9198,7 @@
         <v>7</v>
       </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="61"/>
+      <c r="G16" s="52"/>
       <c r="H16" s="5"/>
       <c r="I16" s="1" t="s">
         <v>6</v>
@@ -9201,7 +9207,7 @@
         <v>7</v>
       </c>
       <c r="K16" s="3"/>
-      <c r="L16" s="61"/>
+      <c r="L16" s="52"/>
       <c r="M16" s="5"/>
       <c r="N16" s="1" t="s">
         <v>6</v>
@@ -9210,7 +9216,7 @@
         <v>7</v>
       </c>
       <c r="P16" s="3"/>
-      <c r="Q16" s="61"/>
+      <c r="Q16" s="52"/>
       <c r="R16" s="5"/>
       <c r="S16" s="1" t="s">
         <v>6</v>
@@ -9220,7 +9226,7 @@
       </c>
     </row>
     <row r="17" spans="2:20">
-      <c r="B17" s="57"/>
+      <c r="B17" s="65"/>
       <c r="C17" s="5" t="s">
         <v>2</v>
       </c>
@@ -9231,7 +9237,7 @@
         <v>601</v>
       </c>
       <c r="F17" s="3"/>
-      <c r="G17" s="61"/>
+      <c r="G17" s="52"/>
       <c r="H17" s="5" t="s">
         <v>2</v>
       </c>
@@ -9242,7 +9248,7 @@
         <v>603</v>
       </c>
       <c r="K17" s="3"/>
-      <c r="L17" s="61"/>
+      <c r="L17" s="52"/>
       <c r="M17" s="5" t="s">
         <v>2</v>
       </c>
@@ -9253,7 +9259,7 @@
         <v>605</v>
       </c>
       <c r="P17" s="3"/>
-      <c r="Q17" s="61"/>
+      <c r="Q17" s="52"/>
       <c r="R17" s="5" t="s">
         <v>2</v>
       </c>
@@ -9265,7 +9271,7 @@
       </c>
     </row>
     <row r="18" spans="2:20">
-      <c r="B18" s="57"/>
+      <c r="B18" s="65"/>
       <c r="C18" s="5" t="s">
         <v>3</v>
       </c>
@@ -9276,7 +9282,7 @@
         <v>149</v>
       </c>
       <c r="F18" s="3"/>
-      <c r="G18" s="61"/>
+      <c r="G18" s="52"/>
       <c r="H18" s="5" t="s">
         <v>3</v>
       </c>
@@ -9287,7 +9293,7 @@
         <v>209</v>
       </c>
       <c r="K18" s="3"/>
-      <c r="L18" s="61"/>
+      <c r="L18" s="52"/>
       <c r="M18" s="5" t="s">
         <v>3</v>
       </c>
@@ -9298,7 +9304,7 @@
         <v>269</v>
       </c>
       <c r="P18" s="3"/>
-      <c r="Q18" s="61"/>
+      <c r="Q18" s="52"/>
       <c r="R18" s="5" t="s">
         <v>3</v>
       </c>
@@ -9310,7 +9316,7 @@
       </c>
     </row>
     <row r="19" spans="2:20">
-      <c r="B19" s="57"/>
+      <c r="B19" s="65"/>
       <c r="C19" s="5" t="s">
         <v>4</v>
       </c>
@@ -9321,7 +9327,7 @@
         <v>151</v>
       </c>
       <c r="F19" s="3"/>
-      <c r="G19" s="61"/>
+      <c r="G19" s="52"/>
       <c r="H19" s="5" t="s">
         <v>4</v>
       </c>
@@ -9332,7 +9338,7 @@
         <v>211</v>
       </c>
       <c r="K19" s="3"/>
-      <c r="L19" s="61"/>
+      <c r="L19" s="52"/>
       <c r="M19" s="5" t="s">
         <v>4</v>
       </c>
@@ -9343,7 +9349,7 @@
         <v>271</v>
       </c>
       <c r="P19" s="3"/>
-      <c r="Q19" s="61"/>
+      <c r="Q19" s="52"/>
       <c r="R19" s="5" t="s">
         <v>4</v>
       </c>
@@ -9355,28 +9361,28 @@
       </c>
     </row>
     <row r="20" spans="2:20">
-      <c r="B20" s="57"/>
+      <c r="B20" s="65"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="4"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="61"/>
+      <c r="G20" s="52"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="4"/>
       <c r="K20" s="3"/>
-      <c r="L20" s="61"/>
+      <c r="L20" s="52"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="4"/>
       <c r="P20" s="3"/>
-      <c r="Q20" s="61"/>
+      <c r="Q20" s="52"/>
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
       <c r="T20" s="17"/>
     </row>
     <row r="21" spans="2:20">
-      <c r="B21" s="57"/>
+      <c r="B21" s="65"/>
       <c r="C21" s="6" t="s">
         <v>9</v>
       </c>
@@ -9385,7 +9391,7 @@
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="61"/>
+      <c r="G21" s="52"/>
       <c r="H21" s="6" t="s">
         <v>9</v>
       </c>
@@ -9394,7 +9400,7 @@
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="3"/>
-      <c r="L21" s="61"/>
+      <c r="L21" s="52"/>
       <c r="M21" s="6" t="s">
         <v>9</v>
       </c>
@@ -9403,7 +9409,7 @@
       </c>
       <c r="O21" s="8"/>
       <c r="P21" s="3"/>
-      <c r="Q21" s="61"/>
+      <c r="Q21" s="52"/>
       <c r="R21" s="6" t="s">
         <v>9</v>
       </c>
@@ -9413,7 +9419,7 @@
       <c r="T21" s="21"/>
     </row>
     <row r="22" spans="2:20">
-      <c r="B22" s="58"/>
+      <c r="B22" s="66"/>
       <c r="C22" s="9" t="s">
         <v>25</v>
       </c>
@@ -9424,7 +9430,7 @@
         <v>24</v>
       </c>
       <c r="F22" s="3"/>
-      <c r="G22" s="62"/>
+      <c r="G22" s="53"/>
       <c r="H22" s="9" t="s">
         <v>25</v>
       </c>
@@ -9435,7 +9441,7 @@
         <v>24</v>
       </c>
       <c r="K22" s="3"/>
-      <c r="L22" s="62"/>
+      <c r="L22" s="53"/>
       <c r="M22" s="9" t="s">
         <v>25</v>
       </c>
@@ -9446,7 +9452,7 @@
         <v>24</v>
       </c>
       <c r="P22" s="3"/>
-      <c r="Q22" s="62"/>
+      <c r="Q22" s="53"/>
       <c r="R22" s="9" t="s">
         <v>25</v>
       </c>
@@ -9568,7 +9574,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="2:20" ht="17.25" thickBot="1">
+    <row r="26" spans="2:20" ht="15.75" thickBot="1">
       <c r="B26" s="23"/>
       <c r="C26" s="24"/>
       <c r="D26" s="25"/>
@@ -9825,11 +9831,11 @@
       <c r="N39" s="49">
         <v>1</v>
       </c>
-      <c r="O39" s="66" t="s">
+      <c r="O39" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="P39" s="66"/>
-      <c r="Q39" s="66"/>
+      <c r="P39" s="50"/>
+      <c r="Q39" s="50"/>
     </row>
     <row r="40" spans="3:17">
       <c r="H40" s="38" t="s">
@@ -9847,11 +9853,11 @@
       <c r="N40" s="49">
         <v>2</v>
       </c>
-      <c r="O40" s="66" t="s">
+      <c r="O40" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="P40" s="66"/>
-      <c r="Q40" s="66"/>
+      <c r="P40" s="50"/>
+      <c r="Q40" s="50"/>
     </row>
     <row r="41" spans="3:17">
       <c r="H41" s="38"/>
@@ -9867,11 +9873,11 @@
       <c r="N41" s="49">
         <v>3</v>
       </c>
-      <c r="O41" s="66" t="s">
+      <c r="O41" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="P41" s="66"/>
-      <c r="Q41" s="66"/>
+      <c r="P41" s="50"/>
+      <c r="Q41" s="50"/>
     </row>
     <row r="42" spans="3:17">
       <c r="H42" s="47" t="s">
@@ -9919,12 +9925,20 @@
         <v>56</v>
       </c>
     </row>
+    <row r="47" spans="3:17">
+      <c r="I47" t="s">
+        <v>82</v>
+      </c>
+    </row>
     <row r="48" spans="3:17">
       <c r="C48" s="14" t="s">
         <v>15</v>
       </c>
       <c r="D48" t="s">
         <v>80</v>
+      </c>
+      <c r="I48" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="4:4">
@@ -9934,12 +9948,20 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="O39:Q39"/>
-    <mergeCell ref="O40:Q40"/>
-    <mergeCell ref="O41:Q41"/>
-    <mergeCell ref="L14:L22"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="Q14:Q22"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B4:B12"/>
+    <mergeCell ref="B14:B22"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="G4:G12"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="G14:G22"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
     <mergeCell ref="S14:T14"/>
     <mergeCell ref="N15:O15"/>
     <mergeCell ref="S15:T15"/>
@@ -9951,20 +9973,12 @@
     <mergeCell ref="S4:T4"/>
     <mergeCell ref="N5:O5"/>
     <mergeCell ref="S5:T5"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="G4:G12"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="G14:G22"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B4:B12"/>
-    <mergeCell ref="B14:B22"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="O39:Q39"/>
+    <mergeCell ref="O40:Q40"/>
+    <mergeCell ref="O41:Q41"/>
+    <mergeCell ref="L14:L22"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="Q14:Q22"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9980,7 +9994,7 @@
       <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>